<commit_message>
The Q1 is almost done! - 3 columns is not defined yet!
</commit_message>
<xml_diff>
--- a/Q1.xlsx
+++ b/Q1.xlsx
@@ -8,14 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="order_data" sheetId="2" r:id="rId2"/>
+    <sheet name="Order_data" sheetId="2" r:id="rId2"/>
+    <sheet name="Comments" sheetId="3" r:id="rId3"/>
+    <sheet name="Orders" sheetId="4" r:id="rId4"/>
+    <sheet name="Quality" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="74">
   <si>
     <t>نام ویژگی</t>
   </si>
@@ -83,6 +86,9 @@
     <t>TODO</t>
   </si>
   <si>
+    <t>topOutliers: 729321.75 - downOutliers: 721123.75</t>
+  </si>
+  <si>
     <t>product_variant_id</t>
   </si>
   <si>
@@ -123,6 +129,117 @@
   </si>
   <si>
     <t>marketplace_seller_id</t>
+  </si>
+  <si>
+    <t>topOutliers: 23679104.25 - downOutliers: 6269424.25</t>
+  </si>
+  <si>
+    <t>topOutliers: 2089106.5 - downOutliers: 832622.5</t>
+  </si>
+  <si>
+    <t>topOutliers: 18169750.0 - downOutliers: -9749850.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 18302500.0 - downOutliers: -9717500.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 6.0 - downOutliers: -2.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 1.0 - downOutliers: 1.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 0.0 - downOutliers: 0.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 1177822.5 - downOutliers: -484565.5</t>
+  </si>
+  <si>
+    <t>topOutliers: 131040.0 - downOutliers: -77672.0</t>
+  </si>
+  <si>
+    <t>confirmed_at</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>topOutliers: 888108.0 - downOutliers: -215556.0</t>
+  </si>
+  <si>
+    <t>ID_Order</t>
+  </si>
+  <si>
+    <t>ID_Customer</t>
+  </si>
+  <si>
+    <t>ID_Item</t>
+  </si>
+  <si>
+    <t>DateTime_CartFinalize</t>
+  </si>
+  <si>
+    <t>Amount_Gross_Order</t>
+  </si>
+  <si>
+    <t>city_name_fa</t>
+  </si>
+  <si>
+    <t>Quantity_item</t>
+  </si>
+  <si>
+    <t>topOutliers: 23617535.875 - downOutliers: -6134917.125</t>
+  </si>
+  <si>
+    <t>topOutliers: 8916465.5 - downOutliers: -3716194.5</t>
+  </si>
+  <si>
+    <t>topOutliers: 1163831.0 - downOutliers: -555007.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 2345671.125 - downOutliers: -1213365.875</t>
+  </si>
+  <si>
+    <t>product_title</t>
+  </si>
+  <si>
+    <t>title_en</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>likes</t>
+  </si>
+  <si>
+    <t>dislikes</t>
+  </si>
+  <si>
+    <t>verification_status</t>
+  </si>
+  <si>
+    <t>recommend</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>advantages</t>
+  </si>
+  <si>
+    <t>disadvantages</t>
+  </si>
+  <si>
+    <t>topOutliers: 1180373.0 - downOutliers: -371483.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 13863722.25 - downOutliers: -4166585.75</t>
+  </si>
+  <si>
+    <t>topOutliers: 10.0 - downOutliers: -6.0</t>
+  </si>
+  <si>
+    <t>topOutliers: 5.0 - downOutliers: -3.0</t>
   </si>
 </sst>
 </file>
@@ -544,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -566,9 +683,6 @@
       <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
@@ -589,9 +703,6 @@
       <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
@@ -612,9 +723,6 @@
       <c r="I5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -635,9 +743,6 @@
       <c r="I6" t="s">
         <v>21</v>
       </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
@@ -658,9 +763,6 @@
       <c r="I7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
@@ -681,9 +783,6 @@
       <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
@@ -704,9 +803,6 @@
       <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
@@ -727,9 +823,6 @@
       <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -748,9 +841,6 @@
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -825,7 +915,7 @@
         <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -833,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -857,7 +947,7 @@
         <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -865,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -889,7 +979,7 @@
         <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -897,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -921,7 +1011,7 @@
         <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -929,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -941,9 +1031,6 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -952,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -964,9 +1051,6 @@
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -975,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -999,7 +1083,7 @@
         <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1007,7 +1091,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1019,9 +1103,6 @@
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1030,7 +1111,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1042,9 +1123,6 @@
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1053,7 +1131,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -1065,9 +1143,6 @@
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1076,7 +1151,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -1100,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1108,7 +1183,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -1132,7 +1207,7 @@
         <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1140,7 +1215,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1152,9 +1227,6 @@
         <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1163,7 +1235,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1187,7 +1259,7 @@
         <v>21</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1195,7 +1267,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1219,6 +1291,692 @@
         <v>21</v>
       </c>
       <c r="J16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>281</v>
+      </c>
+      <c r="F2">
+        <v>684859</v>
+      </c>
+      <c r="G2">
+        <v>333613.6409817523</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>1000411</v>
+      </c>
+      <c r="F2">
+        <v>24846558</v>
+      </c>
+      <c r="G2">
+        <v>9871963.252730001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>466132</v>
+      </c>
+      <c r="F3">
+        <v>7282118</v>
+      </c>
+      <c r="G3">
+        <v>2860671.082805</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>76</v>
+      </c>
+      <c r="F4">
+        <v>2093722</v>
+      </c>
+      <c r="G4">
+        <v>375731.267395</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1530000000</v>
+      </c>
+      <c r="G6">
+        <v>1458204.043815</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>500</v>
+      </c>
+      <c r="G8">
+        <v>1.261225</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>908917</v>
+      </c>
+      <c r="G2">
+        <v>412510.3731623932</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>466132</v>
+      </c>
+      <c r="F5">
+        <v>8623288</v>
+      </c>
+      <c r="G5">
+        <v>4669121.762427351</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>495</v>
+      </c>
+      <c r="G6">
+        <v>3.45165811965812</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1344</v>
+      </c>
+      <c r="G7">
+        <v>1.979042735042735</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The Q1 is almost done! - wait for fatemeh to check it
</commit_message>
<xml_diff>
--- a/Q1.xlsx
+++ b/Q1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
   <si>
     <t>نام ویژگی</t>
   </si>
@@ -83,7 +83,34 @@
     <t>object</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>From 723112.0 to 727967.0</t>
+  </si>
+  <si>
+    <t>کیف پول زنانه چرم دیبا کد Z2</t>
+  </si>
+  <si>
+    <t>simplewears</t>
+  </si>
+  <si>
+    <t>کاور-سانتا-باربارا-مدل-black-lable-مناسب-برای-گوشی-موبایل-آیفون-6-6s</t>
+  </si>
+  <si>
+    <t>تابلو بوم نقاشی، نقاشی کلاسیک، تابلو مدرن، قاب عکس، دکوراسیون داخلی، تابلو خط، تابلو خوشنویسی، شاسی ام دی اف، نقاشی قدیمی، تابلو چاپی، تابلو شاسی، بوم</t>
+  </si>
+  <si>
+    <t>کیف و کاور گوشی</t>
+  </si>
+  <si>
+    <t>کیف و کاور گوشی Cell-Phone-Pouch-Cover</t>
+  </si>
+  <si>
+    <t>متفرقه</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>[{"Key":"سایر توضیحات","Value":"چاپ بر روي پارچه بوم وارداتي مات ضدآب و با رنگ هاي بدون بو و حساسيت\r\nكلاف چهارچوب ساخته شده از چوب سبک روس سفيد با پهناي ديپ چهار سانتي متر\r\nقابليت شستشو با پارچه نرم مرطوب"},{"Key":"جنس","Value":"چوب"},{"Key":"کشور مبداء برند","Value":"ایران"},{"Key":"وزن","Value":"1200 \/ 1800"},{"Key":"ابعاد","Value":"سایز یک : 50x70  سایز دو 100x70"},{"Key":"حالت استفاده","Value":"آویز"}]</t>
   </si>
   <si>
     <t>topOutliers: 729321.75 - downOutliers: 721123.75</t>
@@ -131,6 +158,33 @@
     <t>marketplace_seller_id</t>
   </si>
   <si>
+    <t>From 7003798.0 to 18752077.0</t>
+  </si>
+  <si>
+    <t>From 1155042.0 to 1977385.0</t>
+  </si>
+  <si>
+    <t>From 1.0 to 1.2500012000012e+17</t>
+  </si>
+  <si>
+    <t>From 0.0 to 14500.0</t>
+  </si>
+  <si>
+    <t>From 0.0 to 1.0</t>
+  </si>
+  <si>
+    <t>From 300.0 to 957891.0</t>
+  </si>
+  <si>
+    <t>From 1.0 to 90731.0</t>
+  </si>
+  <si>
+    <t>\N</t>
+  </si>
+  <si>
+    <t>2018-10-09 09:39:31</t>
+  </si>
+  <si>
     <t>topOutliers: 23679104.25 - downOutliers: 6269424.25</t>
   </si>
   <si>
@@ -164,6 +218,15 @@
     <t>comment</t>
   </si>
   <si>
+    <t>From 281.0 to 684859.0</t>
+  </si>
+  <si>
+    <t>2018-04-20 09:19:37</t>
+  </si>
+  <si>
+    <t>عالی</t>
+  </si>
+  <si>
     <t>topOutliers: 888108.0 - downOutliers: -215556.0</t>
   </si>
   <si>
@@ -188,6 +251,27 @@
     <t>Quantity_item</t>
   </si>
   <si>
+    <t>From 1000411.0 to 24846558.0</t>
+  </si>
+  <si>
+    <t>From 466132.0 to 7282118.0</t>
+  </si>
+  <si>
+    <t>From 76.0 to 2093722.0</t>
+  </si>
+  <si>
+    <t>From 0.0 to 1530000000.0</t>
+  </si>
+  <si>
+    <t>From 1.0 to 500.0</t>
+  </si>
+  <si>
+    <t>2016-05-17 17:40:25.000</t>
+  </si>
+  <si>
+    <t>تهران</t>
+  </si>
+  <si>
     <t>topOutliers: 23617535.875 - downOutliers: -6134917.125</t>
   </si>
   <si>
@@ -228,6 +312,36 @@
   </si>
   <si>
     <t>disadvantages</t>
+  </si>
+  <si>
+    <t>From 300.0 to 908917.0</t>
+  </si>
+  <si>
+    <t>From 466132.0 to 8623288.0</t>
+  </si>
+  <si>
+    <t>From 0.0 to 495.0</t>
+  </si>
+  <si>
+    <t>From 0.0 to 1344.0</t>
+  </si>
+  <si>
+    <t>مچ بند هوشمند شیائومی مدل Mi Band 2</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>recommended</t>
+  </si>
+  <si>
+    <t>عالیه</t>
+  </si>
+  <si>
+    <t>["ندارد"]</t>
   </si>
   <si>
     <t>topOutliers: 1180373.0 - downOutliers: -371483.0</t>
@@ -654,14 +768,11 @@
       <c r="G2">
         <v>725372.183908046</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
+      <c r="I2">
+        <v>725474.5</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -674,14 +785,8 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -694,14 +799,8 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -714,14 +813,8 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -734,14 +827,8 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
       <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -754,14 +841,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -774,14 +855,8 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -794,14 +869,8 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -814,14 +883,8 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
       <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -834,14 +897,8 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>7003798</v>
@@ -908,14 +965,11 @@
       <c r="G2">
         <v>14856496.22150078</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
+      <c r="I2">
+        <v>15349798</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -923,13 +977,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>1155042</v>
@@ -940,14 +994,11 @@
       <c r="G3">
         <v>1474217.296549375</v>
       </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+      <c r="I3">
+        <v>1434234</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -955,13 +1006,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -972,14 +1023,11 @@
       <c r="G4">
         <v>58350651358.43367</v>
       </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
+      <c r="I4">
+        <v>3436000</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -987,13 +1035,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1004,14 +1052,11 @@
       <c r="G5">
         <v>58525940918.38041</v>
       </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
+      <c r="I5">
+        <v>3500000</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1019,19 +1064,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
       <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1039,19 +1078,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1059,13 +1092,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1076,14 +1109,11 @@
       <c r="G8">
         <v>5.127288200926771</v>
       </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
+      <c r="I8">
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1091,19 +1121,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1111,19 +1135,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
       <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1131,19 +1149,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1151,13 +1163,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1168,14 +1180,11 @@
       <c r="G12">
         <v>0.9980987548744299</v>
       </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
+      <c r="I12">
+        <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1183,13 +1192,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1200,14 +1209,11 @@
       <c r="G13">
         <v>0.06230709434991883</v>
       </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
+      <c r="I13">
+        <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1215,19 +1221,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
       <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1235,13 +1235,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>300</v>
@@ -1252,14 +1252,11 @@
       <c r="G15">
         <v>346268.3136830135</v>
       </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
+      <c r="I15">
+        <v>290328</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1267,13 +1264,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1284,14 +1281,11 @@
       <c r="G16">
         <v>20622.4126278751</v>
       </c>
-      <c r="H16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" t="s">
-        <v>21</v>
+      <c r="I16">
+        <v>8251</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1341,13 +1335,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="E2">
         <v>281</v>
@@ -1358,14 +1352,11 @@
       <c r="G2">
         <v>333613.6409817523</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
+      <c r="I2">
+        <v>342220</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1373,19 +1364,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1393,19 +1378,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1455,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>1000411</v>
@@ -1472,14 +1451,11 @@
       <c r="G2">
         <v>9871963.252730001</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
+      <c r="I2">
+        <v>8591270</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1487,13 +1463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>466132</v>
@@ -1504,14 +1480,11 @@
       <c r="G3">
         <v>2860671.082805</v>
       </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+      <c r="I3">
+        <v>2895180.5</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1519,13 +1492,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>76</v>
@@ -1536,14 +1509,11 @@
       <c r="G4">
         <v>375731.267395</v>
       </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
+      <c r="I4">
+        <v>230221</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1551,19 +1521,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1571,13 +1535,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1588,14 +1552,11 @@
       <c r="G6">
         <v>1458204.043815</v>
       </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
+      <c r="I6">
+        <v>321101</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1603,19 +1564,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1623,13 +1578,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1640,14 +1595,11 @@
       <c r="G8">
         <v>1.261225</v>
       </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
+      <c r="I8">
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1697,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="E2">
         <v>300</v>
@@ -1714,14 +1666,11 @@
       <c r="G2">
         <v>412510.3731623932</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
+      <c r="I2">
+        <v>405146.5</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1729,19 +1678,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1749,19 +1692,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1769,13 +1706,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E5">
         <v>466132</v>
@@ -1786,14 +1723,11 @@
       <c r="G5">
         <v>4669121.762427351</v>
       </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
+      <c r="I5">
+        <v>4862451.5</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1801,13 +1735,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1818,14 +1752,11 @@
       <c r="G6">
         <v>3.45165811965812</v>
       </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
+      <c r="I6">
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1833,13 +1764,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1850,14 +1781,11 @@
       <c r="G7">
         <v>1.979042735042735</v>
       </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
+      <c r="I7">
+        <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1865,19 +1793,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1885,19 +1807,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1905,19 +1821,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
       <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1925,19 +1835,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1945,19 +1849,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
       <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1965,19 +1863,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
       <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The Q1 completed :) Akh jooon
</commit_message>
<xml_diff>
--- a/Q1.xlsx
+++ b/Q1.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\7th term\DataMining\Proj\Data-Mining-on-DigiKala-dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="Order_data" sheetId="2" r:id="rId2"/>
+    <sheet name="Order_date" sheetId="2" r:id="rId2"/>
     <sheet name="Comments" sheetId="3" r:id="rId3"/>
     <sheet name="Orders" sheetId="4" r:id="rId4"/>
     <sheet name="Quality" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="118">
   <si>
     <t>نام ویژگی</t>
   </si>
@@ -86,13 +91,13 @@
     <t>From 723112.0 to 727967.0</t>
   </si>
   <si>
-    <t>کیف پول زنانه چرم دیبا کد Z2</t>
+    <t>کاور سانتا باربارا مدل Black Lable مناسب برای گوشی موبایل آیفون 6 / 6s</t>
   </si>
   <si>
     <t>simplewears</t>
   </si>
   <si>
-    <t>کاور-سانتا-باربارا-مدل-black-lable-مناسب-برای-گوشی-موبایل-آیفون-6-6s</t>
+    <t>کیف-پول-زنانه-چرم-دیبا-کد-z2</t>
   </si>
   <si>
     <t>تابلو بوم نقاشی، نقاشی کلاسیک، تابلو مدرن، قاب عکس، دکوراسیون داخلی، تابلو خط، تابلو خوشنویسی، شاسی ام دی اف، نقاشی قدیمی، تابلو چاپی، تابلو شاسی، بوم</t>
@@ -134,12 +139,6 @@
     <t>order_limit</t>
   </si>
   <si>
-    <t>start_at</t>
-  </si>
-  <si>
-    <t>end_at</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
@@ -149,15 +148,30 @@
     <t>active</t>
   </si>
   <si>
-    <t>created_at</t>
-  </si>
-  <si>
     <t>product_id</t>
   </si>
   <si>
     <t>marketplace_seller_id</t>
   </si>
   <si>
+    <t>start_at_time</t>
+  </si>
+  <si>
+    <t>start_at_date</t>
+  </si>
+  <si>
+    <t>end_at_time</t>
+  </si>
+  <si>
+    <t>end_at_date</t>
+  </si>
+  <si>
+    <t>created_at_time</t>
+  </si>
+  <si>
+    <t>created_at_date</t>
+  </si>
+  <si>
     <t>From 7003798.0 to 18752077.0</t>
   </si>
   <si>
@@ -179,10 +193,13 @@
     <t>From 1.0 to 90731.0</t>
   </si>
   <si>
-    <t>\N</t>
-  </si>
-  <si>
-    <t>2018-10-09 09:39:31</t>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>09:39:31</t>
   </si>
   <si>
     <t>topOutliers: 23679104.25 - downOutliers: 6269424.25</t>
@@ -212,21 +229,24 @@
     <t>topOutliers: 131040.0 - downOutliers: -77672.0</t>
   </si>
   <si>
-    <t>confirmed_at</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
+    <t>confirmed_at_time</t>
+  </si>
+  <si>
+    <t>confirmed_at_date</t>
+  </si>
+  <si>
     <t>From 281.0 to 684859.0</t>
   </si>
   <si>
-    <t>2018-04-20 09:19:37</t>
-  </si>
-  <si>
     <t>عالی</t>
   </si>
   <si>
+    <t>09:19:37</t>
+  </si>
+  <si>
     <t>topOutliers: 888108.0 - downOutliers: -215556.0</t>
   </si>
   <si>
@@ -239,9 +259,6 @@
     <t>ID_Item</t>
   </si>
   <si>
-    <t>DateTime_CartFinalize</t>
-  </si>
-  <si>
     <t>Amount_Gross_Order</t>
   </si>
   <si>
@@ -251,6 +268,12 @@
     <t>Quantity_item</t>
   </si>
   <si>
+    <t>DateTime_CartFinalize_time</t>
+  </si>
+  <si>
+    <t>DateTime_CartFinalize_date</t>
+  </si>
+  <si>
     <t>From 1000411.0 to 24846558.0</t>
   </si>
   <si>
@@ -266,10 +289,10 @@
     <t>From 1.0 to 500.0</t>
   </si>
   <si>
-    <t>2016-05-17 17:40:25.000</t>
-  </si>
-  <si>
     <t>تهران</t>
+  </si>
+  <si>
+    <t>17:32:36</t>
   </si>
   <si>
     <t>topOutliers: 23617535.875 - downOutliers: -6134917.125</t>
@@ -359,8 +382,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,17 +438,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -469,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +536,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,6 +571,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -710,14 +747,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="61.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -766,7 +814,7 @@
         <v>727967</v>
       </c>
       <c r="G2">
-        <v>725372.183908046</v>
+        <v>725372.18390804599</v>
       </c>
       <c r="I2">
         <v>725474.5</v>
@@ -775,7 +823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -789,7 +837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -803,7 +851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -817,7 +865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -831,7 +879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -845,7 +893,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -859,7 +907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -873,7 +921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -887,7 +935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -907,14 +955,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="44.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,7 +999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -954,7 +1010,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>7003798</v>
@@ -969,10 +1025,10 @@
         <v>15349798</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -983,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>1155042</v>
@@ -992,16 +1048,16 @@
         <v>1977385</v>
       </c>
       <c r="G3">
-        <v>1474217.296549375</v>
+        <v>1474217.2965493749</v>
       </c>
       <c r="I3">
         <v>1434234</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1012,7 +1068,7 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1027,10 +1083,10 @@
         <v>3436000</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1041,7 +1097,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1050,16 +1106,16 @@
         <v>1.2500012000012E+17</v>
       </c>
       <c r="G5">
-        <v>58525940918.38041</v>
+        <v>58525940918.380409</v>
       </c>
       <c r="I5">
         <v>3500000</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1069,11 +1125,8 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1083,11 +1136,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1098,7 +1148,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1107,16 +1157,16 @@
         <v>14500</v>
       </c>
       <c r="G8">
-        <v>5.127288200926771</v>
+        <v>5.1272882009267713</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1126,11 +1176,8 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1138,13 +1185,28 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.99809875487442989</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1152,13 +1214,28 @@
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>6.230709434991883E-2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1169,25 +1246,25 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>957891</v>
       </c>
       <c r="G12">
-        <v>0.9980987548744299</v>
+        <v>346268.31368301349</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>290328</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1198,25 +1275,25 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>90731</v>
       </c>
       <c r="G13">
-        <v>0.06230709434991883</v>
+        <v>20622.412627875099</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>8251</v>
       </c>
       <c r="J13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1227,10 +1304,10 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1238,28 +1315,13 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15">
-        <v>300</v>
-      </c>
-      <c r="F15">
-        <v>957891</v>
-      </c>
-      <c r="G15">
-        <v>346268.3136830135</v>
-      </c>
-      <c r="I15">
-        <v>290328</v>
-      </c>
-      <c r="J15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>20</v>
+      </c>
+      <c r="H15" s="2">
+        <v>43351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1267,25 +1329,52 @@
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>90731</v>
-      </c>
-      <c r="G16">
-        <v>20622.4126278751</v>
-      </c>
-      <c r="I16">
-        <v>8251</v>
-      </c>
-      <c r="J16" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="2">
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="2">
+        <v>43421</v>
       </c>
     </row>
   </sheetData>
@@ -1294,14 +1383,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="10" max="10" width="42.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,18 +1426,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E2">
         <v>281</v>
@@ -1350,41 +1446,55 @@
         <v>684859</v>
       </c>
       <c r="G2">
-        <v>333613.6409817523</v>
+        <v>333613.64098175231</v>
       </c>
       <c r="I2">
         <v>342220</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
+        <v>43194</v>
       </c>
     </row>
   </sheetData>
@@ -1393,14 +1503,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="48.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1429,18 +1544,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>1000411</v>
@@ -1449,27 +1564,27 @@
         <v>24846558</v>
       </c>
       <c r="G2">
-        <v>9871963.252730001</v>
+        <v>9871963.2527300008</v>
       </c>
       <c r="I2">
         <v>8591270</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>466132</v>
@@ -1478,27 +1593,27 @@
         <v>7282118</v>
       </c>
       <c r="G3">
-        <v>2860671.082805</v>
+        <v>2860671.0828049998</v>
       </c>
       <c r="I3">
         <v>2895180.5</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E4">
         <v>76</v>
@@ -1507,99 +1622,113 @@
         <v>2093722</v>
       </c>
       <c r="G4">
-        <v>375731.267395</v>
+        <v>375731.26739499997</v>
       </c>
       <c r="I4">
         <v>230221</v>
       </c>
       <c r="J4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1530000000</v>
+      </c>
+      <c r="G5">
+        <v>1458204.043815</v>
+      </c>
+      <c r="I5">
+        <v>321101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1530000000</v>
-      </c>
-      <c r="G6">
-        <v>1458204.043815</v>
-      </c>
-      <c r="I6">
-        <v>321101</v>
-      </c>
-      <c r="J6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>1.261225</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
-      <c r="G8">
-        <v>1.261225</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2">
+        <v>43088</v>
       </c>
     </row>
   </sheetData>
@@ -1608,14 +1737,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" customWidth="1"/>
+    <col min="10" max="10" width="45.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1644,18 +1782,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E2">
         <v>300</v>
@@ -1664,55 +1802,55 @@
         <v>908917</v>
       </c>
       <c r="G2">
-        <v>412510.3731623932</v>
+        <v>412510.37316239323</v>
       </c>
       <c r="I2">
         <v>405146.5</v>
       </c>
       <c r="J2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E5">
         <v>466132</v>
@@ -1721,27 +1859,27 @@
         <v>8623288</v>
       </c>
       <c r="G5">
-        <v>4669121.762427351</v>
+        <v>4669121.7624273514</v>
       </c>
       <c r="I5">
         <v>4862451.5</v>
       </c>
       <c r="J5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1756,21 +1894,21 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1779,97 +1917,97 @@
         <v>1344</v>
       </c>
       <c r="G7">
-        <v>1.979042735042735</v>
+        <v>1.9790427350427351</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>